<commit_message>
Add shopping description; reduce price
</commit_message>
<xml_diff>
--- a/const/shopping_list.xlsx
+++ b/const/shopping_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="31540" windowHeight="17360" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3480" yWindow="580" windowWidth="31540" windowHeight="17360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="宝石" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>商品类型</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -272,6 +272,78 @@
   </si>
   <si>
     <t>1 FREE lottery per day, double protection time for a month</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文描述</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文描述</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机获得一个品质的恐龙蛋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机获得一个高品质的恐龙蛋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get a dinosaur egg by random</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get a high quality egg by random</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加恐龙的速度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加恐龙的防御力</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加恐龙的HP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加宝物的掉率</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加经验获得</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗中增加恐龙的攻击力</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase dinosaurs' speed in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase dinosaurs' attack in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase dinosaurs' defense in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase dinosaurs' HP in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase experience in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increase treasure dropping in battle</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -279,8 +351,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -397,7 +470,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="54">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -452,8 +525,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,8 +578,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="54">
+  <cellStyles count="60">
     <cellStyle name="标题" xfId="1" builtinId="15"/>
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
@@ -528,6 +608,9 @@
     <cellStyle name="超链接" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
@@ -554,6 +637,9 @@
     <cellStyle name="访问过的超链接" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,7 +977,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M2" sqref="M2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -955,8 +1041,8 @@
       <c r="C2" s="3">
         <v>1001</v>
       </c>
-      <c r="D2" s="3">
-        <v>255</v>
+      <c r="D2">
+        <v>400</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>59</v>
@@ -974,11 +1060,11 @@
       <c r="J2" s="4"/>
       <c r="K2" s="8">
         <f>D2/G2</f>
-        <v>51.102204408817634</v>
+        <v>80.160320641282567</v>
       </c>
       <c r="L2" s="8">
         <f>D2/H2</f>
-        <v>8.5</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16">
@@ -991,8 +1077,8 @@
       <c r="C3" s="3">
         <v>1002</v>
       </c>
-      <c r="D3" s="3">
-        <v>600</v>
+      <c r="D3">
+        <v>900</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>52</v>
@@ -1010,11 +1096,11 @@
       <c r="J3" s="4"/>
       <c r="K3" s="8">
         <f t="shared" ref="K3:K6" si="0">D3/G3</f>
-        <v>60.06006006006006</v>
+        <v>90.090090090090087</v>
       </c>
       <c r="L3" s="8">
         <f t="shared" ref="L3:L6" si="1">D3/H3</f>
-        <v>8.8235294117647065</v>
+        <v>13.235294117647058</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16">
@@ -1027,8 +1113,8 @@
       <c r="C4" s="3">
         <v>1003</v>
       </c>
-      <c r="D4" s="3">
-        <v>1250</v>
+      <c r="D4">
+        <v>2000</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>53</v>
@@ -1046,11 +1132,11 @@
       <c r="J4" s="4"/>
       <c r="K4" s="8">
         <f t="shared" si="0"/>
-        <v>62.531265632816414</v>
+        <v>100.05002501250627</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="1"/>
-        <v>9.765625</v>
+        <v>15.625</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16">
@@ -1063,8 +1149,8 @@
       <c r="C5" s="3">
         <v>1004</v>
       </c>
-      <c r="D5" s="3">
-        <v>3300</v>
+      <c r="D5">
+        <v>5000</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>51</v>
@@ -1082,11 +1168,11 @@
       <c r="J5" s="4"/>
       <c r="K5" s="8">
         <f t="shared" si="0"/>
-        <v>66.013202640528107</v>
+        <v>100.02000400080016</v>
       </c>
       <c r="L5" s="8">
         <f t="shared" si="1"/>
-        <v>10.060975609756097</v>
+        <v>15.24390243902439</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16">
@@ -1099,8 +1185,8 @@
       <c r="C6" s="3">
         <v>1005</v>
       </c>
-      <c r="D6" s="3">
-        <v>7000</v>
+      <c r="D6">
+        <v>12000</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>54</v>
@@ -1118,11 +1204,11 @@
       <c r="J6" s="4"/>
       <c r="K6" s="8">
         <f t="shared" si="0"/>
-        <v>70.007000700070009</v>
+        <v>120.01200120012003</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" si="1"/>
-        <v>10.802469135802468</v>
+        <v>18.518518518518519</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1507,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H2" sqref="H2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1521,7 +1607,7 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:9" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1630,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1563,11 +1649,13 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="17">
+        <v>120</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1586,11 +1674,13 @@
       <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" s="17">
+        <v>150</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1609,11 +1699,13 @@
       <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="3">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="17">
+        <v>187.5</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1632,11 +1724,13 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="3">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="17">
+        <v>240</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1655,11 +1749,13 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="17">
+        <v>300</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1678,11 +1774,13 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="17">
+        <v>375</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1701,11 +1799,13 @@
       <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="3">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="17">
+        <v>240</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1724,11 +1824,13 @@
       <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="G9" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="17">
+        <v>300</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1747,9 +1849,11 @@
       <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="3">
-        <v>250</v>
-      </c>
+      <c r="G10" s="17">
+        <v>375</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1765,19 +1869,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="11" style="1"/>
+    <col min="8" max="8" width="50.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="59.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21">
+    <row r="1" spans="1:15" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1799,26 +1905,32 @@
       <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1832,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1840,26 +1952,32 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="14">
+      <c r="K2" s="14">
         <v>0.3</v>
       </c>
-      <c r="J2" s="14">
+      <c r="L2" s="14">
         <v>0.39</v>
       </c>
-      <c r="K2" s="14">
+      <c r="M2" s="14">
         <v>0.2</v>
       </c>
-      <c r="L2" s="15">
+      <c r="N2" s="15">
         <v>0.1099</v>
       </c>
-      <c r="M2" s="15">
+      <c r="O2" s="15">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1873,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="10">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1881,26 +1999,32 @@
       <c r="G3" s="1">
         <v>2</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="14">
+      <c r="K3" s="14">
         <v>0</v>
       </c>
-      <c r="J3" s="14">
-        <v>0.6</v>
-      </c>
-      <c r="K3" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="L3" s="15">
+      <c r="L3" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="15">
         <v>9.9900000000000003E-2</v>
       </c>
-      <c r="M3" s="15">
+      <c r="O3" s="15">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1914,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -1922,8 +2046,14 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="H4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1937,7 +2067,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
@@ -1945,14 +2075,20 @@
       <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1966,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
@@ -1974,14 +2110,20 @@
       <c r="G6" s="1">
         <v>3</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="H6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1995,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
@@ -2003,14 +2145,20 @@
       <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="H7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2024,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1">
         <v>3</v>
@@ -2032,14 +2180,20 @@
       <c r="G8" s="1">
         <v>5</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="H8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2053,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
@@ -2061,14 +2215,20 @@
       <c r="G9" s="1">
         <v>6</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2082,7 +2242,7 @@
         <v>200</v>
       </c>
       <c r="E10" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
@@ -2090,14 +2250,16 @@
       <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -2111,7 +2273,7 @@
         <v>200</v>
       </c>
       <c r="E11" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3">
         <v>2</v>
@@ -2119,14 +2281,16 @@
       <c r="G11" s="3">
         <v>2</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -2140,7 +2304,7 @@
         <v>200</v>
       </c>
       <c r="E12" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
@@ -2148,8 +2312,10 @@
       <c r="G12" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2329,7 @@
         <v>200</v>
       </c>
       <c r="E13" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
@@ -2171,8 +2337,10 @@
       <c r="G13" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -2186,7 +2354,7 @@
         <v>200</v>
       </c>
       <c r="E14" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
@@ -2194,8 +2362,10 @@
       <c r="G14" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2379,7 @@
         <v>200</v>
       </c>
       <c r="E15" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F15" s="3">
         <v>2</v>
@@ -2217,8 +2387,10 @@
       <c r="G15" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -2232,7 +2404,7 @@
         <v>200</v>
       </c>
       <c r="E16" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
@@ -2240,8 +2412,10 @@
       <c r="G16" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -2255,7 +2429,7 @@
         <v>200</v>
       </c>
       <c r="E17" s="10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3">
         <v>2</v>
@@ -2263,6 +2437,8 @@
       <c r="G17" s="3">
         <v>8</v>
       </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2280,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2334,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>600</v>
+        <v>199</v>
       </c>
       <c r="F2" s="1">
         <v>4</v>
@@ -2392,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>6</v>

</xml_diff>

<commit_message>
Add gems reward desc
</commit_message>
<xml_diff>
--- a/const/shopping_list.xlsx
+++ b/const/shopping_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="580" windowWidth="31540" windowHeight="17360" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="20" windowWidth="35300" windowHeight="17920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="宝石" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>商品类型</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -344,6 +344,54 @@
   </si>
   <si>
     <t>Increase treasure dropping in battle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>en</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次购买赠送白色霸王龙*1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次购买赠送10万金币</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次购买赠送绿色霸王龙*1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次购买赠送紫色霸王龙*1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次购买赠送蓝色霸王龙*1和蓝色震龙*1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First-time-purchase: 100k gold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First-time-purchase: white Tyrent x 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First-time-purchase: green Tyrent x 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First-time-purchase: purple Tyrent x 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First-time-purchase: blue Tyrent x 1, blue earthquake x 1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -974,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -991,9 +1039,11 @@
     <col min="9" max="9" width="11" style="1"/>
     <col min="10" max="10" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5" customWidth="1"/>
+    <col min="14" max="14" width="57.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="21">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="21">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -1030,8 +1080,14 @@
       <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16">
+      <c r="M1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1066,8 +1122,14 @@
         <f>D2/H2</f>
         <v>13.333333333333334</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16">
+      <c r="M2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1102,8 +1164,14 @@
         <f t="shared" ref="L3:L6" si="1">D3/H3</f>
         <v>14.705882352941176</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16">
+      <c r="M3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1138,8 +1206,14 @@
         <f t="shared" si="1"/>
         <v>16.40625</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16">
+      <c r="M4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1174,8 +1248,14 @@
         <f t="shared" si="1"/>
         <v>16.76829268292683</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16">
+      <c r="M5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1210,8 +1290,14 @@
         <f t="shared" si="1"/>
         <v>18.518518518518519</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1219,7 +1305,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1227,7 +1313,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1235,7 +1321,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1243,7 +1329,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1251,7 +1337,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14">
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1259,7 +1345,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1267,7 +1353,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1275,7 +1361,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1283,7 +1369,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14">
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>

</xml_diff>

<commit_message>
Try new battle code
</commit_message>
<xml_diff>
--- a/const/shopping_list.xlsx
+++ b/const/shopping_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2940" yWindow="0" windowWidth="29620" windowHeight="17200" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="宝石" sheetId="1" r:id="rId1"/>
@@ -255,14 +255,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>每日登录即获得一张抽奖券；保护时间加倍；持续一月</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 FREE lottery per day, double protection time for a month</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>中文描述</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -416,6 +408,14 @@
   </si>
   <si>
     <t>Increase experience 15%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日登录额外获得一张抽奖券；保护时间加倍；额外赠送一次攻打巢穴的次数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extra FREE lottery per day, double protection time; extra chance to attack cave</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1254,10 +1254,10 @@
         <v>29</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16">
@@ -1296,10 +1296,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16">
@@ -1338,10 +1338,10 @@
         <v>22.058823529411764</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="16">
@@ -1380,10 +1380,10 @@
         <v>24.21875</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16">
@@ -1422,10 +1422,10 @@
         <v>24.390243902439025</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16">
@@ -1464,10 +1464,10 @@
         <v>27.777777777777779</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1882,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -2162,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2196,10 +2196,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>12</v>
@@ -2208,20 +2208,20 @@
         <v>13</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="Q1" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R1" s="28"/>
       <c r="S1" s="28"/>
@@ -2259,7 +2259,7 @@
         <v>39</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -2289,7 +2289,7 @@
         <v>9</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -2316,10 +2316,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K3" s="27">
         <v>0.3</v>
@@ -2396,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K4" s="27">
         <v>0</v>
@@ -2476,10 +2476,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="K5" s="27">
         <v>0</v>
@@ -2556,10 +2556,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -2586,10 +2586,10 @@
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2622,10 +2622,10 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
@@ -2658,10 +2658,10 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -2694,10 +2694,10 @@
         <v>11</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -2730,10 +2730,10 @@
         <v>12</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2995,8 +2995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3058,10 +3058,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9">

</xml_diff>

<commit_message>
Fix aps and iap
</commit_message>
<xml_diff>
--- a/const/shopping_list.xlsx
+++ b/const/shopping_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="0" windowWidth="29620" windowHeight="17200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3880" yWindow="0" windowWidth="29620" windowHeight="17200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="宝石" sheetId="1" r:id="rId1"/>
@@ -204,21 +204,6 @@
     <t>DINO_STYLE_GEM_USD_4999</t>
   </si>
   <si>
-    <t>com.dinosaur.gems.usd4999</t>
-  </si>
-  <si>
-    <t>com.dinosaur.gems.usd999</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.dinosaur.gems.usd1999</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.dinosaur.gems.usd9999</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>DINO_STYLE_GEM_USD_9999</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -235,10 +220,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>com.dinosaur.gems.usd499</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>抽取更好的奖品</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -416,6 +397,25 @@
   </si>
   <si>
     <t>Extra FREE lottery per day, double protection time; extra chance to attack cave</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.gaofei.dinostyle2.gems.us499</t>
+  </si>
+  <si>
+    <t>com.gaofei.dinostyle2.gems.us999</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.gaofei.dinostyle2.gems.us1999</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.gaofei.dinostyle2.gems.us4999</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.gaofei.dinostyle2.gems.us9999</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1254,10 +1254,10 @@
         <v>29</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16">
@@ -1274,10 +1274,10 @@
         <v>600</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G2" s="6">
         <v>4.99</v>
@@ -1296,10 +1296,10 @@
         <v>20</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16">
@@ -1316,10 +1316,10 @@
         <v>1500</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G3" s="6">
         <v>9.99</v>
@@ -1338,10 +1338,10 @@
         <v>22.058823529411764</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="16">
@@ -1358,10 +1358,10 @@
         <v>3100</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G4" s="6">
         <v>19.989999999999998</v>
@@ -1380,10 +1380,10 @@
         <v>24.21875</v>
       </c>
       <c r="M4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16">
@@ -1400,7 +1400,7 @@
         <v>8000</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>47</v>
@@ -1422,10 +1422,10 @@
         <v>24.390243902439025</v>
       </c>
       <c r="M5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16">
@@ -1442,10 +1442,10 @@
         <v>18000</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G6" s="6">
         <v>99.99</v>
@@ -1464,10 +1464,10 @@
         <v>27.777777777777779</v>
       </c>
       <c r="M6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1882,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -2196,10 +2196,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>12</v>
@@ -2208,20 +2208,20 @@
         <v>13</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="Q1" s="28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="R1" s="28"/>
       <c r="S1" s="28"/>
@@ -2259,7 +2259,7 @@
         <v>39</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -2289,7 +2289,7 @@
         <v>9</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -2316,10 +2316,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K3" s="27">
         <v>0.3</v>
@@ -2396,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K4" s="27">
         <v>0</v>
@@ -2476,10 +2476,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K5" s="27">
         <v>0</v>
@@ -2556,10 +2556,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -2586,10 +2586,10 @@
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2622,10 +2622,10 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
@@ -2658,10 +2658,10 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -2694,10 +2694,10 @@
         <v>11</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -2730,10 +2730,10 @@
         <v>12</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2995,7 +2995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -3058,10 +3058,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3145,10 +3145,10 @@
         <v>2</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3174,10 +3174,10 @@
         <v>3</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>